<commit_message>
prepare ana final test case for development
</commit_message>
<xml_diff>
--- a/data/TD_NGQ_CPQ_EncoreRetirement_US9400_ItemActions_08.xlsx
+++ b/data/TD_NGQ_CPQ_EncoreRetirement_US9400_ItemActions_08.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>OpportunityID</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>LineItemSelector</t>
+  </si>
+  <si>
+    <t>ProductNumber</t>
+  </si>
+  <si>
+    <t>G3U45A</t>
   </si>
 </sst>
 </file>
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,14 +426,15 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -444,32 +451,38 @@
         <v>0</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pushing US9400_08 for review
</commit_message>
<xml_diff>
--- a/data/TD_NGQ_CPQ_EncoreRetirement_US9400_ItemActions_08.xlsx
+++ b/data/TD_NGQ_CPQ_EncoreRetirement_US9400_ItemActions_08.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>OpportunityID</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>LineItemSelector</t>
+  </si>
+  <si>
+    <t>ProductNumber</t>
+  </si>
+  <si>
+    <t>G3U45A</t>
   </si>
 </sst>
 </file>
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,14 +426,15 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -444,32 +451,38 @@
         <v>0</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit new script: Func_AssignGroupName
</commit_message>
<xml_diff>
--- a/data/TD_NGQ_CPQ_EncoreRetirement_US9400_ItemActions_08.xlsx
+++ b/data/TD_NGQ_CPQ_EncoreRetirement_US9400_ItemActions_08.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ngq-demo-develop\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>OpportunityID</t>
   </si>
@@ -72,6 +67,12 @@
   </si>
   <si>
     <t>G3U45A</t>
+  </si>
+  <si>
+    <t>BaseProduct</t>
+  </si>
+  <si>
+    <t>U8LQ2E</t>
   </si>
 </sst>
 </file>
@@ -405,7 +406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -413,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +435,7 @@
     <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -468,8 +469,11 @@
       <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
@@ -484,6 +488,9 @@
       </c>
       <c r="J2" t="s">
         <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>